<commit_message>
bottom dashtable is formatted nicely tried adjusting style.css to make dropdowns play nice corrected the lat lon for "Near Mumbain coast"
</commit_message>
<xml_diff>
--- a/cleaned_ports_list.xlsx
+++ b/cleaned_ports_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Khorfakkan Port, Sharjah, UAE</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>Near Mumbai coast</t>
   </si>
 </sst>
 </file>
@@ -555,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,8 +1566,23 @@
         <v>55.325795999516998</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67" si="1">A67&amp;"~"&amp;B67&amp;"~"&amp;C67</f>
+        <f t="shared" ref="D67:D68" si="1">A67&amp;"~"&amp;B67&amp;"~"&amp;C67</f>
         <v>Anchorage outside Dubai, UAE~25.3593799592826~55.325795999517</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="1">
+        <v>19.084793478010301</v>
+      </c>
+      <c r="C68" s="1">
+        <v>72.870532634994007</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>Near Mumbai coast~19.0847934780103~72.870532634994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>